<commit_message>
Added in Order related pages and service methods, made minor updates to functionality
</commit_message>
<xml_diff>
--- a/Requirements.xlsx
+++ b/Requirements.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dan.G\source\repos\RestaurantDemoApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E1135A0E-83CA-491A-94D3-915DE63AA2BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9004EC5-BEA0-42CF-94F0-774C8334C827}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6420" yWindow="2790" windowWidth="21600" windowHeight="11385"/>
+    <workbookView xWindow="5175" yWindow="1815" windowWidth="21600" windowHeight="11400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="54">
   <si>
     <t>Restaurant Demo</t>
   </si>
@@ -126,9 +126,6 @@
     <t>Completed</t>
   </si>
   <si>
-    <t>In Progress</t>
-  </si>
-  <si>
     <t>Use @onchange and @onSelectionchange events on the table for updating values</t>
   </si>
   <si>
@@ -147,14 +144,65 @@
     <t>Tip</t>
   </si>
   <si>
-    <t xml:space="preserve">Mainly Complete. Need to add tipping </t>
+    <t>change error message for Customer Name</t>
+  </si>
+  <si>
+    <t>Add Delete options for Inventory and discount code</t>
+  </si>
+  <si>
+    <t>Mainly Complete. Need to add tipping  and discount</t>
+  </si>
+  <si>
+    <t>Hard Type roles</t>
+  </si>
+  <si>
+    <t>Id field is 0 when saving and updating without calling to db</t>
+  </si>
+  <si>
+    <t>Add clickable fields for table headers to sort using lists. Add boolean trigger to switch</t>
+  </si>
+  <si>
+    <t>Not implemented</t>
+  </si>
+  <si>
+    <t>Next in line</t>
+  </si>
+  <si>
+    <t>Discount Codes don't expire automatically. Need to add a quick trigger to activate or deactivate a coupon</t>
+  </si>
+  <si>
+    <t>Create a coupon model for validation</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Discount percentage as well as cost </t>
+  </si>
+  <si>
+    <t>Discount code activation should show message to user. Needs to reduce the number of uses as well</t>
+  </si>
+  <si>
+    <t>Reduce inventory for order</t>
+  </si>
+  <si>
+    <t>Proper Clear function</t>
+  </si>
+  <si>
+    <t>Add images with scrolling</t>
+  </si>
+  <si>
+    <t>Show orders to complete, with an option to mark as completed</t>
+  </si>
+  <si>
+    <t>ADD in the user name by default when placing order</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -202,13 +250,20 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -222,7 +277,24 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
@@ -268,7 +340,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="8">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -277,8 +349,11 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -286,18 +361,18 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="5"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="2" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="3"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="6"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="7"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="7" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="8"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="10"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="10" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="3" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="6" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="8" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="10" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyAlignment="1">
@@ -306,10 +381,24 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="4" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="9" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="6" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="7" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="7"/>
   </cellXfs>
-  <cellStyles count="8">
-    <cellStyle name="60% - Accent6" xfId="7" builtinId="52"/>
-    <cellStyle name="Accent6" xfId="6" builtinId="49"/>
+  <cellStyles count="11">
+    <cellStyle name="20% - Accent1" xfId="7" builtinId="30"/>
+    <cellStyle name="40% - Accent6" xfId="9" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="10" builtinId="52"/>
+    <cellStyle name="Accent6" xfId="8" builtinId="49"/>
+    <cellStyle name="Bad" xfId="6" builtinId="27"/>
     <cellStyle name="Good" xfId="5" builtinId="26"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Heading 2" xfId="2" builtinId="17"/>
@@ -626,23 +715,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="49.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="58.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.7109375" customWidth="1"/>
     <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -650,8 +739,11 @@
         <v>20</v>
       </c>
       <c r="F1" s="3"/>
-    </row>
-    <row r="2" spans="1:7" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>27</v>
       </c>
@@ -668,10 +760,13 @@
         <v>21</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>2</v>
       </c>
@@ -682,14 +777,16 @@
         <v>16</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="5"/>
+      <c r="B4" s="5" t="s">
+        <v>51</v>
+      </c>
       <c r="C4" s="9" t="s">
         <v>29</v>
       </c>
@@ -703,7 +800,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>7</v>
       </c>
@@ -721,7 +818,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E6" s="2" t="s">
         <v>15</v>
       </c>
@@ -732,7 +829,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
@@ -740,7 +837,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>17</v>
@@ -750,7 +847,7 @@
       </c>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -760,32 +857,40 @@
       </c>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
         <v>9</v>
+      </c>
+      <c r="B9" s="15"/>
+      <c r="C9" s="14" t="s">
+        <v>42</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F10" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="16" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="17"/>
+      <c r="C12" s="16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>4</v>
       </c>
@@ -794,16 +899,16 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="5"/>
+      <c r="C14" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>19</v>
       </c>
@@ -812,19 +917,82 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16"/>
+      <c r="C16"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>33</v>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>